<commit_message>
TOOLS-SE FINAL OKTOBER 2023
</commit_message>
<xml_diff>
--- a/public/file/FORMAT_TOOL_EXCEL.xlsx
+++ b/public/file/FORMAT_TOOL_EXCEL.xlsx
@@ -19,77 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
-  <si>
-    <t>rute</t>
-  </si>
-  <si>
-    <t>hari</t>
-  </si>
-  <si>
-    <t>rute id</t>
-  </si>
-  <si>
-    <t>id mrdo</t>
-  </si>
-  <si>
-    <t>survey pasar id</t>
-  </si>
-  <si>
-    <t>SELASA</t>
-  </si>
-  <si>
-    <t>00001/10625282</t>
-  </si>
-  <si>
-    <t>TOKO NAHYA JAYA</t>
-  </si>
-  <si>
-    <t>BLOK C1 NO 3</t>
-  </si>
-  <si>
-    <t>PASAR CIGUDEG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Kode Customer</t>
   </si>
   <si>
-    <t>Nama Toko</t>
-  </si>
-  <si>
-    <t>Alamat</t>
-  </si>
-  <si>
-    <t>id pasar</t>
-  </si>
-  <si>
-    <t>nama pasar</t>
-  </si>
-  <si>
-    <t>Pasar</t>
-  </si>
-  <si>
-    <t>Lokasi</t>
-  </si>
-  <si>
-    <t>salesman</t>
-  </si>
-  <si>
-    <t> BGR MI AGUS ABDILAH B2</t>
-  </si>
-  <si>
     <t>wilayah</t>
   </si>
   <si>
-    <t>BOGOR</t>
-  </si>
-  <si>
-    <t>rute detail id</t>
-  </si>
-  <si>
-    <t>RABU</t>
-  </si>
-  <si>
     <t>Salesman Tujuan</t>
   </si>
   <si>
@@ -97,6 +34,21 @@
   </si>
   <si>
     <t>Hari Tujuan</t>
+  </si>
+  <si>
+    <t>SURABAYA 1</t>
+  </si>
+  <si>
+    <t>999-0044829</t>
+  </si>
+  <si>
+    <t>OFFICE2 </t>
+  </si>
+  <si>
+    <t>JUMAT GENAP</t>
+  </si>
+  <si>
+    <t>JUMAT</t>
   </si>
 </sst>
 </file>
@@ -125,12 +77,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,10 +105,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,134 +389,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="54" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" customWidth="1"/>
-    <col min="14" max="14" width="54" customWidth="1"/>
-    <col min="15" max="15" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2">
-        <v>361</v>
-      </c>
-      <c r="F2" s="2">
-        <v>56869</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1624838</v>
-      </c>
-      <c r="H2" s="2">
-        <v>50212</v>
-      </c>
-      <c r="I2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2">
-        <v>1771</v>
-      </c>
-      <c r="M2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TOOLS-SE FINAL DESEMBER 2023
</commit_message>
<xml_diff>
--- a/public/file/FORMAT_TOOL_EXCEL.xlsx
+++ b/public/file/FORMAT_TOOL_EXCEL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk.widyanto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\api-se\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Kode Customer</t>
   </si>
@@ -49,6 +52,9 @@
   </si>
   <si>
     <t>JUMAT</t>
+  </si>
+  <si>
+    <t>Id wilayah</t>
   </si>
 </sst>
 </file>
@@ -64,6 +70,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -103,12 +110,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,60 +401,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8">
+      <c r="A2" s="4">
+        <v>201</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="2"/>
-      <c r="G7" s="2"/>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update terbaru Tool Excel
</commit_message>
<xml_diff>
--- a/public/file/FORMAT_TOOL_EXCEL.xlsx
+++ b/public/file/FORMAT_TOOL_EXCEL.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Kode Customer</t>
   </si>
@@ -52,13 +52,16 @@
   </si>
   <si>
     <t>JUMAT</t>
+  </si>
+  <si>
+    <t>Id wilayah</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -398,61 +401,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>11</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="B1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>